<commit_message>
change file fiin directly
</commit_message>
<xml_diff>
--- a/ETL/vietnames_to_fiin.xlsx
+++ b/ETL/vietnames_to_fiin.xlsx
@@ -5,13 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quanghung20gg/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quanghung20gg/code/fs_chatbot/chatbot_financial_statement/ETL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E391F7C-652F-9A49-AAD2-86ADF031970A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D2EED8-B245-3D4D-9BAC-DA7CF571104F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="1040" windowWidth="16860" windowHeight="19500" firstSheet="5" activeTab="11" xr2:uid="{181F491C-CE5D-4C83-A516-210AAAD12FF4}"/>
-    <workbookView xWindow="17180" yWindow="1040" windowWidth="16880" windowHeight="19520" firstSheet="1" activeTab="8" xr2:uid="{E372F426-2869-E24D-8798-A3AF32536E4D}"/>
+    <workbookView xWindow="2980" yWindow="500" windowWidth="22380" windowHeight="26080" firstSheet="3" activeTab="3" xr2:uid="{181F491C-CE5D-4C83-A516-210AAAD12FF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Standard BS" sheetId="4" r:id="rId1"/>
@@ -54,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7964" uniqueCount="3270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7970" uniqueCount="3271">
   <si>
     <t>vi_caption</t>
   </si>
@@ -9864,6 +9863,9 @@
   </si>
   <si>
     <t>TM_108</t>
+  </si>
+  <si>
+    <t>Nợ phải trả ngắn hạn</t>
   </si>
 </sst>
 </file>
@@ -10596,9 +10598,6 @@
     <sheetView topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
-    <sheetView topLeftCell="A119" zoomScale="110" zoomScaleNormal="110" workbookViewId="1">
-      <selection activeCell="D144" sqref="D144"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
@@ -15219,7 +15218,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
-    <sheetView topLeftCell="A78" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
@@ -19002,9 +19000,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="E145" sqref="E145"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="G106" sqref="G106:G109"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
@@ -22022,10 +22017,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68BDE7DB-271F-48AD-B868-DC80D2A870AC}">
   <dimension ref="A1:H643"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C411" workbookViewId="0">
+    <sheetView topLeftCell="C411" workbookViewId="0">
       <selection activeCell="G438" sqref="G438"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
@@ -23242,7 +23236,7 @@
         <v>66</v>
       </c>
       <c r="D67" t="str">
-        <f t="shared" ref="D67:E130" si="1">_xlfn.CONCAT("TM_",C67)</f>
+        <f t="shared" ref="D67:D130" si="1">_xlfn.CONCAT("TM_",C67)</f>
         <v>TM_66</v>
       </c>
       <c r="G67" s="30" t="s">
@@ -33739,9 +33733,6 @@
     <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="H77" sqref="H77"/>
     </sheetView>
-    <sheetView topLeftCell="A26" workbookViewId="1">
-      <selection activeCell="B45" sqref="B45"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
@@ -33835,7 +33826,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="28">
+    <row r="4" spans="1:9" ht="30">
       <c r="A4" s="25"/>
       <c r="B4" s="24"/>
       <c r="C4" s="25" t="s">
@@ -33877,7 +33868,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="28">
+    <row r="6" spans="1:9" ht="30">
       <c r="A6" s="25"/>
       <c r="B6" s="24"/>
       <c r="C6" s="25" t="s">
@@ -33898,7 +33889,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="28">
+    <row r="7" spans="1:9" ht="30">
       <c r="A7" s="25"/>
       <c r="B7" s="24"/>
       <c r="C7" s="25" t="s">
@@ -33919,7 +33910,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="28">
+    <row r="8" spans="1:9" ht="30">
       <c r="A8" s="25"/>
       <c r="B8" s="24"/>
       <c r="C8" s="25" t="s">
@@ -33940,7 +33931,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="28">
+    <row r="9" spans="1:9" ht="30">
       <c r="A9" s="25"/>
       <c r="B9" s="24"/>
       <c r="C9" s="25" t="s">
@@ -33982,7 +33973,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="28">
+    <row r="11" spans="1:9" ht="30">
       <c r="A11" s="25"/>
       <c r="B11" s="24"/>
       <c r="C11" s="25" t="s">
@@ -34024,7 +34015,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" ht="30">
       <c r="A13" s="25"/>
       <c r="B13" s="24"/>
       <c r="C13" s="25" t="s">
@@ -34129,7 +34120,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="28">
+    <row r="18" spans="1:9" ht="30">
       <c r="A18" s="25" t="s">
         <v>731</v>
       </c>
@@ -34158,7 +34149,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="28">
+    <row r="19" spans="1:9" ht="30">
       <c r="A19" s="25"/>
       <c r="B19" s="24"/>
       <c r="C19" s="25" t="s">
@@ -34200,7 +34191,7 @@
         <v>1676</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="28">
+    <row r="21" spans="1:9" ht="30">
       <c r="A21" s="25"/>
       <c r="B21" s="24"/>
       <c r="C21" s="25" t="s">
@@ -35554,7 +35545,6 @@
     <sheetView topLeftCell="C41" workbookViewId="0">
       <selection activeCell="J72" sqref="J72"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
@@ -35595,7 +35585,7 @@
         <v>3255</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="28">
+    <row r="2" spans="1:11" ht="30">
       <c r="A2" s="26" t="s">
         <v>784</v>
       </c>
@@ -35645,7 +35635,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" ht="30">
       <c r="A4" s="26" t="s">
         <v>786</v>
       </c>
@@ -35670,7 +35660,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="28">
+    <row r="5" spans="1:11" ht="30">
       <c r="A5" s="26" t="s">
         <v>788</v>
       </c>
@@ -35699,7 +35689,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="28">
+    <row r="6" spans="1:11" ht="45">
       <c r="A6" s="26" t="s">
         <v>790</v>
       </c>
@@ -35806,7 +35796,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="28">
+    <row r="10" spans="1:11" ht="30">
       <c r="A10" s="26"/>
       <c r="B10" s="26"/>
       <c r="C10" s="24"/>
@@ -35893,7 +35883,7 @@
       </c>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="1:11" ht="28">
+    <row r="14" spans="1:11" ht="45">
       <c r="A14" s="26" t="s">
         <v>798</v>
       </c>
@@ -35923,7 +35913,7 @@
       </c>
       <c r="K14" s="10"/>
     </row>
-    <row r="15" spans="1:11" ht="28">
+    <row r="15" spans="1:11" ht="30">
       <c r="A15" s="26"/>
       <c r="B15" s="26"/>
       <c r="C15" s="24"/>
@@ -35945,7 +35935,7 @@
       </c>
       <c r="K15" s="10"/>
     </row>
-    <row r="16" spans="1:11" ht="28">
+    <row r="16" spans="1:11" ht="30">
       <c r="A16" s="26"/>
       <c r="B16" s="26"/>
       <c r="C16" s="24"/>
@@ -35989,7 +35979,7 @@
       </c>
       <c r="K17" s="10"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" ht="30">
       <c r="A18" s="26"/>
       <c r="B18" s="26"/>
       <c r="C18" s="24"/>
@@ -36033,7 +36023,7 @@
       </c>
       <c r="K19" s="10"/>
     </row>
-    <row r="20" spans="1:11" ht="28">
+    <row r="20" spans="1:11" ht="30">
       <c r="A20" s="26"/>
       <c r="B20" s="26"/>
       <c r="C20" s="24"/>
@@ -36055,7 +36045,7 @@
       </c>
       <c r="K20" s="10"/>
     </row>
-    <row r="21" spans="1:11" ht="28">
+    <row r="21" spans="1:11" ht="30">
       <c r="A21" s="26"/>
       <c r="B21" s="26"/>
       <c r="C21" s="24"/>
@@ -37441,12 +37431,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBF0D163-580A-4FF7-AAB1-247176513E84}">
-  <dimension ref="A1:E151"/>
+  <dimension ref="A1:E152"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D83" sqref="D2:D83"/>
+    <sheetView tabSelected="1" topLeftCell="A126" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D156" sqref="D156"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14"/>
   <cols>
@@ -37457,7 +37446,7 @@
     <col min="5" max="16384" width="8.6640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" ht="15">
       <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
@@ -37469,7 +37458,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" ht="15">
       <c r="A2" s="1"/>
       <c r="B2" s="10" t="s">
         <v>3</v>
@@ -37482,7 +37471,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" ht="15">
       <c r="A3" s="1"/>
       <c r="B3" s="10" t="s">
         <v>6</v>
@@ -37495,7 +37484,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" ht="30">
       <c r="A4" s="1"/>
       <c r="B4" s="10" t="s">
         <v>9</v>
@@ -37508,7 +37497,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" ht="15">
       <c r="A5" s="1"/>
       <c r="B5" s="10" t="s">
         <v>12</v>
@@ -37521,7 +37510,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" ht="15">
       <c r="A6" s="1"/>
       <c r="B6" s="10" t="s">
         <v>15</v>
@@ -37534,7 +37523,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" ht="30">
       <c r="A7" s="1"/>
       <c r="B7" s="10" t="s">
         <v>18</v>
@@ -37547,7 +37536,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" ht="15">
       <c r="A8" s="1"/>
       <c r="B8" s="10" t="s">
         <v>21</v>
@@ -37560,7 +37549,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" ht="15">
       <c r="A9" s="1"/>
       <c r="B9" s="10" t="s">
         <v>24</v>
@@ -37573,7 +37562,7 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" ht="15">
       <c r="A10" s="1"/>
       <c r="B10" s="10" t="s">
         <v>26</v>
@@ -37586,7 +37575,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" ht="28">
+    <row r="11" spans="1:5" ht="30">
       <c r="A11" s="1"/>
       <c r="B11" s="10" t="s">
         <v>29</v>
@@ -37599,7 +37588,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" ht="15">
       <c r="A12" s="1"/>
       <c r="B12" s="10" t="s">
         <v>32</v>
@@ -37612,7 +37601,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" ht="15">
       <c r="A13" s="1"/>
       <c r="B13" s="10" t="s">
         <v>35</v>
@@ -37625,7 +37614,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" ht="15">
       <c r="A14" s="1"/>
       <c r="B14" s="10" t="s">
         <v>37</v>
@@ -37638,7 +37627,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" ht="15">
       <c r="A15" s="1"/>
       <c r="B15" s="10" t="s">
         <v>40</v>
@@ -37651,7 +37640,7 @@
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" ht="15">
       <c r="A16" s="1"/>
       <c r="B16" s="10" t="s">
         <v>43</v>
@@ -37664,7 +37653,7 @@
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" ht="15">
       <c r="A17" s="1"/>
       <c r="B17" s="10" t="s">
         <v>46</v>
@@ -37677,7 +37666,7 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" ht="30">
       <c r="A18" s="1"/>
       <c r="B18" s="10" t="s">
         <v>49</v>
@@ -37690,7 +37679,7 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" ht="15">
       <c r="A19" s="1"/>
       <c r="B19" s="10" t="s">
         <v>52</v>
@@ -37703,7 +37692,7 @@
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" ht="15">
       <c r="A20" s="1"/>
       <c r="B20" s="10" t="s">
         <v>55</v>
@@ -37716,7 +37705,7 @@
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" ht="15">
       <c r="A21" s="1"/>
       <c r="B21" s="10" t="s">
         <v>58</v>
@@ -37729,7 +37718,7 @@
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" ht="15">
       <c r="A22" s="1"/>
       <c r="B22" s="10" t="s">
         <v>61</v>
@@ -37742,7 +37731,7 @@
       </c>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" ht="15">
       <c r="A23" s="1"/>
       <c r="B23" s="10" t="s">
         <v>64</v>
@@ -37755,7 +37744,7 @@
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" ht="15">
       <c r="A24" s="1"/>
       <c r="B24" s="10" t="s">
         <v>67</v>
@@ -37768,7 +37757,7 @@
       </c>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" ht="15">
       <c r="A25" s="1"/>
       <c r="B25" s="10" t="s">
         <v>70</v>
@@ -37781,7 +37770,7 @@
       </c>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" ht="15">
       <c r="A26" s="1"/>
       <c r="B26" s="10" t="s">
         <v>73</v>
@@ -37794,7 +37783,7 @@
       </c>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" ht="30">
       <c r="A27" s="1"/>
       <c r="B27" s="10" t="s">
         <v>76</v>
@@ -37807,7 +37796,7 @@
       </c>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" ht="15">
       <c r="A28" s="1"/>
       <c r="B28" s="10" t="s">
         <v>79</v>
@@ -37820,7 +37809,7 @@
       </c>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" ht="15">
       <c r="A29" s="1"/>
       <c r="B29" s="10" t="s">
         <v>82</v>
@@ -37833,7 +37822,7 @@
       </c>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" ht="15">
       <c r="A30" s="1"/>
       <c r="B30" s="10" t="s">
         <v>85</v>
@@ -37846,7 +37835,7 @@
       </c>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" ht="15">
       <c r="A31" s="1"/>
       <c r="B31" s="10" t="s">
         <v>88</v>
@@ -37859,7 +37848,7 @@
       </c>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" ht="15">
       <c r="A32" s="1"/>
       <c r="B32" s="10" t="s">
         <v>91</v>
@@ -37872,7 +37861,7 @@
       </c>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" ht="15">
       <c r="A33" s="1"/>
       <c r="B33" s="10" t="s">
         <v>94</v>
@@ -37885,7 +37874,7 @@
       </c>
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" ht="15">
       <c r="A34" s="1"/>
       <c r="B34" s="10" t="s">
         <v>97</v>
@@ -37898,7 +37887,7 @@
       </c>
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" ht="15">
       <c r="A35" s="1"/>
       <c r="B35" s="10" t="s">
         <v>100</v>
@@ -37911,7 +37900,7 @@
       </c>
       <c r="E35" s="2"/>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" ht="15">
       <c r="A36" s="1"/>
       <c r="B36" s="10" t="s">
         <v>103</v>
@@ -37924,7 +37913,7 @@
       </c>
       <c r="E36" s="2"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" ht="15">
       <c r="A37" s="1"/>
       <c r="B37" s="10" t="s">
         <v>106</v>
@@ -37937,7 +37926,7 @@
       </c>
       <c r="E37" s="2"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" ht="15">
       <c r="A38" s="1"/>
       <c r="B38" s="10" t="s">
         <v>109</v>
@@ -37950,7 +37939,7 @@
       </c>
       <c r="E38" s="2"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" ht="15">
       <c r="A39" s="1"/>
       <c r="B39" s="10" t="s">
         <v>112</v>
@@ -37963,7 +37952,7 @@
       </c>
       <c r="E39" s="2"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" ht="15">
       <c r="A40" s="1"/>
       <c r="B40" s="10" t="s">
         <v>115</v>
@@ -39418,6 +39407,17 @@
         <v>449</v>
       </c>
       <c r="E151" s="4"/>
+    </row>
+    <row r="152" spans="1:5" ht="15">
+      <c r="B152" s="10" t="s">
+        <v>3270</v>
+      </c>
+      <c r="C152" s="10" t="s">
+        <v>1595</v>
+      </c>
+      <c r="D152" s="10" t="s">
+        <v>1596</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -39431,7 +39431,6 @@
     <sheetView topLeftCell="A78" workbookViewId="0">
       <selection activeCell="A94" sqref="A94"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
@@ -39496,7 +39495,7 @@
         <v>2146</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28">
+    <row r="5" spans="1:4" ht="30">
       <c r="A5" s="25" t="s">
         <v>9</v>
       </c>
@@ -39538,7 +39537,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="28">
+    <row r="8" spans="1:4" ht="30">
       <c r="A8" s="25" t="s">
         <v>18</v>
       </c>
@@ -39580,7 +39579,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="28">
+    <row r="11" spans="1:4" ht="30">
       <c r="A11" s="25" t="s">
         <v>26</v>
       </c>
@@ -39594,7 +39593,7 @@
         <v>2149</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="28">
+    <row r="12" spans="1:4" ht="30">
       <c r="A12" s="25" t="s">
         <v>29</v>
       </c>
@@ -39720,7 +39719,7 @@
         <v>2153</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="28">
+    <row r="21" spans="1:4" ht="30">
       <c r="A21" s="25" t="s">
         <v>46</v>
       </c>
@@ -39734,7 +39733,7 @@
         <v>2154</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="28">
+    <row r="22" spans="1:4" ht="30">
       <c r="A22" s="25" t="s">
         <v>49</v>
       </c>
@@ -39914,7 +39913,7 @@
         <v>2163</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" ht="30">
       <c r="A35" s="25" t="s">
         <v>94</v>
       </c>
@@ -39928,7 +39927,7 @@
         <v>2164</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="28">
+    <row r="36" spans="1:4" ht="30">
       <c r="A36" s="25" t="s">
         <v>97</v>
       </c>
@@ -40110,7 +40109,7 @@
         <v>2172</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="28">
+    <row r="49" spans="1:4" ht="30">
       <c r="A49" s="25" t="s">
         <v>135</v>
       </c>
@@ -40124,7 +40123,7 @@
         <v>2173</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" ht="30">
       <c r="A50" s="25" t="s">
         <v>222</v>
       </c>
@@ -40152,7 +40151,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="28">
+    <row r="52" spans="1:4" ht="30">
       <c r="A52" s="25" t="s">
         <v>141</v>
       </c>
@@ -40166,7 +40165,7 @@
         <v>2175</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" ht="30">
       <c r="A53" s="25" t="s">
         <v>144</v>
       </c>
@@ -40180,7 +40179,7 @@
         <v>2176</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" ht="30">
       <c r="A54" s="25" t="s">
         <v>147</v>
       </c>
@@ -40222,7 +40221,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="28">
+    <row r="57" spans="1:4" ht="30">
       <c r="A57" s="25" t="s">
         <v>156</v>
       </c>
@@ -40236,7 +40235,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="28">
+    <row r="58" spans="1:4" ht="30">
       <c r="A58" s="25" t="s">
         <v>159</v>
       </c>
@@ -40292,7 +40291,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="28">
+    <row r="62" spans="1:4" ht="30">
       <c r="A62" s="25" t="s">
         <v>171</v>
       </c>
@@ -40320,7 +40319,7 @@
         <v>2180</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="28">
+    <row r="64" spans="1:4" ht="30">
       <c r="A64" s="25" t="s">
         <v>177</v>
       </c>
@@ -40488,7 +40487,7 @@
         <v>2184</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" ht="30">
       <c r="A76" s="25" t="s">
         <v>213</v>
       </c>
@@ -40530,7 +40529,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="28">
+    <row r="79" spans="1:4" ht="30">
       <c r="A79" s="25" t="s">
         <v>246</v>
       </c>
@@ -40600,7 +40599,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="28">
+    <row r="84" spans="1:4" ht="30">
       <c r="A84" s="25" t="s">
         <v>264</v>
       </c>
@@ -40614,7 +40613,7 @@
         <v>2188</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="28">
+    <row r="85" spans="1:4" ht="30">
       <c r="A85" s="25" t="s">
         <v>267</v>
       </c>
@@ -40628,7 +40627,7 @@
         <v>2189</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="28">
+    <row r="86" spans="1:4" ht="30">
       <c r="A86" s="25" t="s">
         <v>270</v>
       </c>
@@ -40724,7 +40723,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="32">
+    <row r="93" spans="1:4" ht="45">
       <c r="A93" s="25" t="s">
         <v>288</v>
       </c>
@@ -41536,7 +41535,6 @@
     <sheetView topLeftCell="A115" workbookViewId="0">
       <selection activeCell="D137" sqref="B1:D179"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
@@ -41638,7 +41636,7 @@
       </c>
       <c r="E7" s="10"/>
     </row>
-    <row r="8" spans="1:5" ht="28">
+    <row r="8" spans="1:5" ht="30">
       <c r="A8" s="9"/>
       <c r="B8" s="10" t="s">
         <v>465</v>
@@ -41716,7 +41714,7 @@
       </c>
       <c r="E13" s="10"/>
     </row>
-    <row r="14" spans="1:5" ht="28">
+    <row r="14" spans="1:5" ht="30">
       <c r="A14" s="9"/>
       <c r="B14" s="10" t="s">
         <v>480</v>
@@ -41859,7 +41857,7 @@
       </c>
       <c r="E24" s="10"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" ht="30">
       <c r="A25" s="9"/>
       <c r="B25" s="10" t="s">
         <v>508</v>
@@ -41872,7 +41870,7 @@
       </c>
       <c r="E25" s="10"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" ht="30">
       <c r="A26" s="9"/>
       <c r="B26" s="10" t="s">
         <v>511</v>
@@ -42197,7 +42195,7 @@
       </c>
       <c r="E50" s="10"/>
     </row>
-    <row r="51" spans="1:5" ht="28">
+    <row r="51" spans="1:5" ht="30">
       <c r="A51" s="9"/>
       <c r="B51" s="10" t="s">
         <v>555</v>
@@ -42340,7 +42338,7 @@
       </c>
       <c r="E61" s="10"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" ht="30">
       <c r="A62" s="9"/>
       <c r="B62" s="10" t="s">
         <v>579</v>
@@ -42496,7 +42494,7 @@
       </c>
       <c r="E73" s="10"/>
     </row>
-    <row r="74" spans="1:5" ht="28">
+    <row r="74" spans="1:5" ht="30">
       <c r="A74" s="9"/>
       <c r="B74" s="10" t="s">
         <v>613</v>
@@ -42587,7 +42585,7 @@
       </c>
       <c r="E80" s="10"/>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" ht="30">
       <c r="A81" s="9"/>
       <c r="B81" s="10" t="s">
         <v>631</v>
@@ -42652,7 +42650,7 @@
       </c>
       <c r="E85" s="10"/>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" ht="30">
       <c r="A86" s="9"/>
       <c r="B86" s="10" t="s">
         <v>644</v>
@@ -42769,7 +42767,7 @@
       </c>
       <c r="E94" s="10"/>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" ht="30">
       <c r="A95" s="9"/>
       <c r="B95" s="10" t="s">
         <v>669</v>
@@ -42821,7 +42819,7 @@
       </c>
       <c r="E98" s="10"/>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" ht="30">
       <c r="A99" s="9"/>
       <c r="B99" s="10" t="s">
         <v>678</v>
@@ -42977,7 +42975,7 @@
       </c>
       <c r="E110" s="10"/>
     </row>
-    <row r="111" spans="1:5" ht="28">
+    <row r="111" spans="1:5" ht="30">
       <c r="A111" s="9"/>
       <c r="B111" s="10" t="s">
         <v>705</v>
@@ -43081,7 +43079,7 @@
       </c>
       <c r="E118" s="10"/>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" ht="30">
       <c r="A119" s="9"/>
       <c r="B119" s="10" t="s">
         <v>727</v>
@@ -43107,7 +43105,7 @@
       </c>
       <c r="E120" s="10"/>
     </row>
-    <row r="121" spans="1:5" ht="28">
+    <row r="121" spans="1:5" ht="30">
       <c r="A121" s="9"/>
       <c r="B121" s="10" t="s">
         <v>731</v>
@@ -43133,7 +43131,7 @@
       </c>
       <c r="E122" s="10"/>
     </row>
-    <row r="123" spans="1:5" ht="28">
+    <row r="123" spans="1:5" ht="30">
       <c r="A123" s="9"/>
       <c r="B123" s="10" t="s">
         <v>735</v>
@@ -43185,7 +43183,7 @@
       </c>
       <c r="E126" s="10"/>
     </row>
-    <row r="127" spans="1:5" ht="28">
+    <row r="127" spans="1:5" ht="30">
       <c r="A127" s="9"/>
       <c r="B127" s="10" t="s">
         <v>743</v>
@@ -43224,7 +43222,7 @@
       </c>
       <c r="E129" s="10"/>
     </row>
-    <row r="130" spans="1:5" ht="28">
+    <row r="130" spans="1:5" ht="30">
       <c r="A130" s="9"/>
       <c r="B130" s="10" t="s">
         <v>752</v>
@@ -43276,7 +43274,7 @@
       </c>
       <c r="E133" s="10"/>
     </row>
-    <row r="134" spans="1:5" ht="28">
+    <row r="134" spans="1:5" ht="30">
       <c r="A134" s="9"/>
       <c r="B134" s="10" t="s">
         <v>763</v>
@@ -43315,7 +43313,7 @@
       </c>
       <c r="E136" s="10"/>
     </row>
-    <row r="137" spans="1:5" ht="28">
+    <row r="137" spans="1:5" ht="30">
       <c r="A137" s="9"/>
       <c r="B137" s="10" t="s">
         <v>770</v>
@@ -43328,7 +43326,7 @@
       </c>
       <c r="E137" s="10"/>
     </row>
-    <row r="138" spans="1:5">
+    <row r="138" spans="1:5" ht="30">
       <c r="A138" s="9"/>
       <c r="B138" s="10" t="s">
         <v>773</v>
@@ -43886,7 +43884,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
@@ -43993,7 +43990,7 @@
         <v>2236</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16">
+    <row r="8" spans="1:4" ht="30">
       <c r="A8" s="25" t="s">
         <v>465</v>
       </c>
@@ -44077,7 +44074,7 @@
         <v>2239</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="28">
+    <row r="14" spans="1:4" ht="30">
       <c r="A14" s="25" t="s">
         <v>480</v>
       </c>
@@ -44231,7 +44228,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16">
+    <row r="25" spans="1:4" ht="30">
       <c r="A25" s="25" t="s">
         <v>508</v>
       </c>
@@ -46420,12 +46417,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCC925B1-2EBA-403C-B6B7-CB6A0F3D3243}">
-  <dimension ref="A1:F190"/>
+  <dimension ref="A1:F191"/>
   <sheetViews>
-    <sheetView topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="C189" sqref="C189"/>
+    <sheetView topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="D191" sqref="C190:D191"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
@@ -46513,7 +46509,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:6" ht="28">
+    <row r="7" spans="1:6" ht="30">
       <c r="A7" s="1"/>
       <c r="B7" s="10" t="s">
         <v>459</v>
@@ -46565,7 +46561,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:6" ht="28">
+    <row r="11" spans="1:6" ht="30">
       <c r="A11" s="1"/>
       <c r="B11" s="10" t="s">
         <v>884</v>
@@ -46604,7 +46600,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:6" ht="28">
+    <row r="14" spans="1:6" ht="30">
       <c r="A14" s="1"/>
       <c r="B14" s="10" t="s">
         <v>893</v>
@@ -46786,7 +46782,7 @@
       </c>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" ht="30">
       <c r="A28" s="1"/>
       <c r="B28" s="10" t="s">
         <v>487</v>
@@ -47176,7 +47172,7 @@
       </c>
       <c r="E57" s="2"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" ht="30">
       <c r="A58" s="1"/>
       <c r="B58" s="10" t="s">
         <v>596</v>
@@ -47280,7 +47276,7 @@
       </c>
       <c r="E65" s="2"/>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" ht="30">
       <c r="A66" s="1"/>
       <c r="B66" s="10" t="s">
         <v>620</v>
@@ -47319,7 +47315,7 @@
       </c>
       <c r="E68" s="2"/>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" ht="30">
       <c r="A69" s="1"/>
       <c r="B69" s="10" t="s">
         <v>151</v>
@@ -47930,7 +47926,7 @@
       </c>
       <c r="E115" s="2"/>
     </row>
-    <row r="116" spans="1:5" ht="28">
+    <row r="116" spans="1:5" ht="30">
       <c r="A116" s="1"/>
       <c r="B116" s="10" t="s">
         <v>403</v>
@@ -48021,7 +48017,7 @@
       </c>
       <c r="E122" s="2"/>
     </row>
-    <row r="123" spans="1:5" ht="28">
+    <row r="123" spans="1:5" ht="30">
       <c r="A123" s="1"/>
       <c r="B123" s="10" t="s">
         <v>857</v>
@@ -48112,7 +48108,7 @@
       </c>
       <c r="E129" s="2"/>
     </row>
-    <row r="130" spans="1:5" ht="28">
+    <row r="130" spans="1:5" ht="30">
       <c r="A130" s="1"/>
       <c r="B130" s="10" t="s">
         <v>1286</v>
@@ -48125,7 +48121,7 @@
       </c>
       <c r="E130" s="2"/>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:5" ht="30">
       <c r="A131" s="1"/>
       <c r="B131" s="10" t="s">
         <v>1288</v>
@@ -48138,7 +48134,7 @@
       </c>
       <c r="E131" s="4"/>
     </row>
-    <row r="132" spans="1:5" ht="28">
+    <row r="132" spans="1:5" ht="30">
       <c r="A132" s="1"/>
       <c r="B132" s="10" t="s">
         <v>247</v>
@@ -48164,7 +48160,7 @@
       </c>
       <c r="E133" s="2"/>
     </row>
-    <row r="134" spans="1:5" ht="28">
+    <row r="134" spans="1:5" ht="30">
       <c r="A134" s="1"/>
       <c r="B134" s="10" t="s">
         <v>1102</v>
@@ -48177,7 +48173,7 @@
       </c>
       <c r="E134" s="2"/>
     </row>
-    <row r="135" spans="1:5" ht="28">
+    <row r="135" spans="1:5" ht="30">
       <c r="A135" s="1"/>
       <c r="B135" s="10" t="s">
         <v>1105</v>
@@ -48190,7 +48186,7 @@
       </c>
       <c r="E135" s="2"/>
     </row>
-    <row r="136" spans="1:5" ht="28">
+    <row r="136" spans="1:5" ht="30">
       <c r="A136" s="1"/>
       <c r="B136" s="10" t="s">
         <v>1108</v>
@@ -48203,7 +48199,7 @@
       </c>
       <c r="E136" s="2"/>
     </row>
-    <row r="137" spans="1:5">
+    <row r="137" spans="1:5" ht="30">
       <c r="A137" s="1"/>
       <c r="B137" s="10" t="s">
         <v>250</v>
@@ -48229,7 +48225,7 @@
       </c>
       <c r="E138" s="2"/>
     </row>
-    <row r="139" spans="1:5" ht="28">
+    <row r="139" spans="1:5" ht="30">
       <c r="A139" s="1"/>
       <c r="B139" s="10" t="s">
         <v>256</v>
@@ -48333,7 +48329,7 @@
       </c>
       <c r="E146" s="2"/>
     </row>
-    <row r="147" spans="1:5" ht="28">
+    <row r="147" spans="1:5" ht="30">
       <c r="A147" s="1"/>
       <c r="B147" s="10" t="s">
         <v>307</v>
@@ -48359,7 +48355,7 @@
       </c>
       <c r="E148" s="2"/>
     </row>
-    <row r="149" spans="1:5" ht="28">
+    <row r="149" spans="1:5" ht="30">
       <c r="A149" s="1"/>
       <c r="B149" s="10" t="s">
         <v>1145</v>
@@ -48372,7 +48368,7 @@
       </c>
       <c r="E149" s="2"/>
     </row>
-    <row r="150" spans="1:5" ht="28">
+    <row r="150" spans="1:5" ht="30">
       <c r="A150" s="1"/>
       <c r="B150" s="10" t="s">
         <v>1148</v>
@@ -48385,7 +48381,7 @@
       </c>
       <c r="E150" s="2"/>
     </row>
-    <row r="151" spans="1:5" ht="28">
+    <row r="151" spans="1:5" ht="30">
       <c r="A151" s="1"/>
       <c r="B151" s="10" t="s">
         <v>1151</v>
@@ -48904,6 +48900,17 @@
         <v>1212</v>
       </c>
       <c r="E190" s="2"/>
+    </row>
+    <row r="191" spans="1:5">
+      <c r="B191" s="10" t="s">
+        <v>780</v>
+      </c>
+      <c r="C191" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="D191" s="10" t="s">
+        <v>834</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F190" xr:uid="{FCC925B1-2EBA-403C-B6B7-CB6A0F3D3243}">
@@ -48922,7 +48929,6 @@
     <sheetView topLeftCell="A114" workbookViewId="0">
       <selection activeCell="C121" sqref="C121"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>

</xml_diff>